<commit_message>
Terminación de consulta temporal e inicio de frontend
</commit_message>
<xml_diff>
--- a/BD_respaldo/Base de Datos Software.xlsx
+++ b/BD_respaldo/Base de Datos Software.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\proyecto\BD_respaldo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764FD407-0ADC-4A06-9014-CF7FADCD5709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC7F33F-1789-49FB-90E1-60098F1C77AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="19770" windowHeight="11760" tabRatio="401" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,13 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
-  <si>
-    <t>categoria_productos</t>
-  </si>
-  <si>
-    <t>id_categoria</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>estado</t>
   </si>
@@ -45,9 +39,6 @@
     <t>nombre_producto</t>
   </si>
   <si>
-    <t>nombre_categoria</t>
-  </si>
-  <si>
     <t>descripcion</t>
   </si>
   <si>
@@ -175,9 +166,6 @@
   </si>
   <si>
     <t>id_producto1</t>
-  </si>
-  <si>
-    <t>id_categoria1</t>
   </si>
   <si>
     <t>id_proveedor1</t>
@@ -837,69 +825,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>372036</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>31853</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1264455</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>62109</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="11 Rombo">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="629771" y="4760735"/>
-          <a:ext cx="892419" cy="590550"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100" b="1"/>
-            <a:t>1:N</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>18</xdr:row>
@@ -1287,13 +1212,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1815353</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>58315</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>556803</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1580,156 +1505,6 @@
             </a:schemeClr>
           </a:solidFill>
         </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>717177</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>91933</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>11207</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="28" name="27 Conector recto">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="974912" y="5918992"/>
-          <a:ext cx="1131795" cy="20126"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>773206</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>818031</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>134470</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="29 Conector recto">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1030941" y="5354131"/>
-          <a:ext cx="44825" cy="607398"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>795619</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>818030</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>37976</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="32" name="31 Conector recto">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1053354" y="4359088"/>
-          <a:ext cx="22411" cy="407770"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="3">
@@ -2345,290 +2120,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>854751</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>69134</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1081885</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>91115</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="59" name="58 Rectángulo">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1112486" y="4450634"/>
-          <a:ext cx="227134" cy="212481"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>N</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1591235</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>168089</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1818369</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>10775</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="59 Rectángulo">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1848970" y="5647765"/>
-          <a:ext cx="227134" cy="212481"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>481853</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>708987</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>44393</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="61" name="60 Rectángulo">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="739588" y="4403912"/>
-          <a:ext cx="227134" cy="212481"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1564342</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1791476</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>6293</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="62" name="61 Rectángulo">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1822077" y="6001871"/>
-          <a:ext cx="227134" cy="212481"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -4943,10 +4434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:J34"/>
+  <dimension ref="B3:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4968,44 +4459,44 @@
   <sheetData>
     <row r="3" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J8" s="8"/>
     </row>
@@ -5014,217 +4505,200 @@
     </row>
     <row r="11" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="E11" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="E12" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="E13" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="E14" s="11" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H15" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="3" t="s">
-        <v>51</v>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="F21" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H21" s="8"/>
       <c r="J21" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
-        <v>34</v>
+      <c r="B22" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H22" s="8"/>
       <c r="J22" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
-        <v>52</v>
+      <c r="B23" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H23" s="8"/>
       <c r="J23" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H24" s="8"/>
     </row>
     <row r="26" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="H26" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="H27" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J27" s="9"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H28" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H29" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H30" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="C31" s="6" t="s">
-        <v>0</v>
-      </c>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H31" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J31" s="8"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C32" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="H32" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C33" s="2" t="s">
-        <v>7</v>
-      </c>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H33" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C34" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>